<commit_message>
29 Sep 2021 Morning
</commit_message>
<xml_diff>
--- a/rundown_matakuliah_IN232_MatDis.xlsx
+++ b/rundown_matakuliah_IN232_MatDis.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="43">
   <si>
     <t xml:space="preserve">Kode Mata Kuliah </t>
   </si>
@@ -104,31 +104,139 @@
     <t xml:space="preserve">Slides Himpunan</t>
   </si>
   <si>
+    <t xml:space="preserve">Diskusi dgn bahas soal bersama2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diskusi tentang Himpunan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.3 Definisi Himpunan &amp; Kesamaan</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">1.4 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Himpunan Bagian</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">1.5 Diagram Venn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.6 Operasi-operasi Himpunan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.7 Kardinalitas Himpunan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.8 Hukum-Hukum Aljabar Himpunan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Relasi &amp; Fungsi Bagian 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Review Soal Pembuktian Himpunan</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">1.2. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Hasil Kali Kartesius</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">Diskusi</t>
   </si>
   <si>
-    <t xml:space="preserve">Diskusi tentang Himpunan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2. Teori Y dan Implementasinya</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.1. ABCD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EFGH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EFGH.pdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IJKL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IJKL.pptx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dst..</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">1.3 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Relasi</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">1.4 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Fungsi</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">1.5 Fungsi Identitas</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">1.6 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Fungsi Satu-ke-satu (One-to-One) </t>
+    </r>
   </si>
 </sst>
 </file>
@@ -138,7 +246,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -170,12 +278,23 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <i val="true"/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -250,6 +369,13 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
       <left style="medium"/>
       <right style="medium"/>
       <top/>
@@ -259,22 +385,15 @@
     <border diagonalUp="false" diagonalDown="false">
       <left style="medium"/>
       <right style="medium"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <top style="medium"/>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left style="medium"/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium"/>
+      <right style="medium"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
   </borders>
@@ -303,7 +422,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="36">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -376,64 +495,76 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="justify" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="justify" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="justify" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -513,17 +644,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="B1:G1048576"/>
+  <dimension ref="B1:G42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B6" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17:C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="1.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="44.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="35.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="35.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="32.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="29.45"/>
@@ -649,21 +780,21 @@
       <c r="D13" s="18" t="n">
         <v>1</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11" t="s">
+      <c r="F13" s="20"/>
+      <c r="G13" s="20" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B14" s="19"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="20" t="n">
-        <v>2</v>
-      </c>
-      <c r="E14" s="21"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="18" t="n">
+        <v>2</v>
+      </c>
+      <c r="E14" s="19"/>
       <c r="F14" s="22" t="s">
         <v>27</v>
       </c>
@@ -671,62 +802,396 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="23" t="s">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B15" s="17"/>
+      <c r="C15" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="24" t="s">
+      <c r="D15" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B16" s="17"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="18" t="n">
+        <v>2</v>
+      </c>
+      <c r="E16" s="19"/>
+      <c r="F16" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="G16" s="22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B17" s="17"/>
+      <c r="C17" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="25" t="n">
-        <v>1</v>
-      </c>
-      <c r="E15" s="26" t="s">
+      <c r="D17" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B18" s="17"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="18" t="n">
+        <v>2</v>
+      </c>
+      <c r="E18" s="19"/>
+      <c r="F18" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="G18" s="22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B19" s="17"/>
+      <c r="C19" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="F15" s="26"/>
-      <c r="G15" s="27" t="s">
+      <c r="D19" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B20" s="17"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="18" t="n">
+        <v>2</v>
+      </c>
+      <c r="E20" s="19"/>
+      <c r="F20" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="G20" s="22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B21" s="17"/>
+      <c r="C21" s="25" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="23"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="28" t="n">
-        <v>2</v>
-      </c>
-      <c r="E16" s="29"/>
-      <c r="F16" s="29" t="s">
+      <c r="D21" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="E21" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B22" s="17"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="18" t="n">
+        <v>2</v>
+      </c>
+      <c r="E22" s="19"/>
+      <c r="F22" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="G22" s="22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B23" s="17"/>
+      <c r="C23" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="G16" s="30" t="s">
+      <c r="D23" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="E23" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B24" s="17"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="18" t="n">
+        <v>2</v>
+      </c>
+      <c r="E24" s="19"/>
+      <c r="F24" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="G24" s="22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B25" s="17"/>
+      <c r="C25" s="25" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="31" t="s">
+      <c r="D25" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="E25" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B26" s="26"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="18" t="n">
+        <v>2</v>
+      </c>
+      <c r="E26" s="19"/>
+      <c r="F26" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="G26" s="22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="32" t="s">
-        <v>35</v>
-      </c>
-      <c r="D17" s="31" t="s">
-        <v>35</v>
-      </c>
-      <c r="E17" s="31" t="s">
-        <v>35</v>
-      </c>
-      <c r="F17" s="31" t="s">
-        <v>35</v>
-      </c>
-      <c r="G17" s="31" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="C27" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D27" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="28"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="14" t="n">
+        <v>2</v>
+      </c>
+      <c r="E28" s="15"/>
+      <c r="F28" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="G28" s="16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="29"/>
+      <c r="C29" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="D29" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="E29" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="F29" s="20"/>
+      <c r="G29" s="20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="31"/>
+      <c r="C30" s="32"/>
+      <c r="D30" s="18" t="n">
+        <v>2</v>
+      </c>
+      <c r="E30" s="19"/>
+      <c r="F30" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="G30" s="22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="31"/>
+      <c r="C31" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="D31" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="E31" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="F31" s="20"/>
+      <c r="G31" s="20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="31"/>
+      <c r="C32" s="32"/>
+      <c r="D32" s="18" t="n">
+        <v>2</v>
+      </c>
+      <c r="E32" s="19"/>
+      <c r="F32" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="G32" s="22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="31"/>
+      <c r="C33" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="D33" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="E33" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="F33" s="20"/>
+      <c r="G33" s="20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="31"/>
+      <c r="C34" s="31"/>
+      <c r="D34" s="18" t="n">
+        <v>2</v>
+      </c>
+      <c r="E34" s="19"/>
+      <c r="F34" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="G34" s="22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="31"/>
+      <c r="C35" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="D35" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="E35" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="F35" s="20"/>
+      <c r="G35" s="20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="31"/>
+      <c r="C36" s="31"/>
+      <c r="D36" s="18" t="n">
+        <v>2</v>
+      </c>
+      <c r="E36" s="19"/>
+      <c r="F36" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="G36" s="22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="31"/>
+      <c r="C37" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="D37" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="E37" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="F37" s="20"/>
+      <c r="G37" s="20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="34"/>
+      <c r="C38" s="31"/>
+      <c r="D38" s="18" t="n">
+        <v>2</v>
+      </c>
+      <c r="E38" s="19"/>
+      <c r="F38" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="G38" s="22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C39" s="33"/>
+      <c r="D39" s="18"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="20"/>
+      <c r="G39" s="20"/>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C40" s="31"/>
+      <c r="D40" s="18"/>
+      <c r="E40" s="19"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="22"/>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C41" s="33"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="19"/>
+      <c r="F41" s="20"/>
+      <c r="G41" s="20"/>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C42" s="35"/>
+      <c r="D42" s="18"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="22"/>
+      <c r="G42" s="22"/>
+    </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="B9:B10"/>

</xml_diff>